<commit_message>
Added Q7, which was missing from the BOM.
</commit_message>
<xml_diff>
--- a/controlSystem/RecoveryBoard/RecoveryBoard-BOM.xlsx
+++ b/controlSystem/RecoveryBoard/RecoveryBoard-BOM.xlsx
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Sheet1"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet2"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sheet2"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sheet3"</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
-  <si>
-    <t>Parts</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
   <si>
     <t>KEMET</t>
   </si>
@@ -54,7 +51,16 @@
     <t>ON Semiconductor</t>
   </si>
   <si>
+    <t>BSS123</t>
+  </si>
+  <si>
     <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>SI7465DP-T1-E3</t>
+  </si>
+  <si>
+    <t>SI7465DP-T1-E3CT-ND</t>
   </si>
 </sst>
 </file>
@@ -118,32 +124,41 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1" shrinkToFit="0" textRotation="0" indent="0"/>
+      <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -154,10 +169,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B1" sqref="B1:B65536"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -169,7 +184,7 @@
     <col min="5" max="5" style="0" width="68.28161057692309" bestFit="1" customWidth="1"/>
     <col min="6" max="6" style="0" width="10.427944711538462" customWidth="1"/>
     <col min="7" max="7" style="0" width="26.14128605769231" bestFit="1" customWidth="1"/>
-    <col min="8" max="256" style="0" width="9.142307692307693"/>
+    <col min="8" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5">
@@ -178,8 +193,10 @@
           <t>Qty</t>
         </is>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Parts</t>
+        </is>
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
@@ -217,7 +234,7 @@
         </is>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -230,7 +247,7 @@
         </is>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -248,7 +265,7 @@
         </is>
       </c>
       <c r="C3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
@@ -261,7 +278,7 @@
         </is>
       </c>
       <c r="F3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
@@ -279,7 +296,7 @@
         </is>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
@@ -292,7 +309,7 @@
         </is>
       </c>
       <c r="F4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="4" t="inlineStr">
         <is>
@@ -310,7 +327,7 @@
         </is>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -323,7 +340,7 @@
         </is>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -341,7 +358,7 @@
         </is>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -354,7 +371,7 @@
         </is>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -387,7 +404,7 @@
         </is>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -420,7 +437,7 @@
         </is>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -438,7 +455,7 @@
         </is>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -451,7 +468,7 @@
         </is>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -469,10 +486,10 @@
         </is>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
@@ -480,10 +497,10 @@
         </is>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="13.5">
@@ -496,10 +513,10 @@
         </is>
       </c>
       <c r="C11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
@@ -507,10 +524,10 @@
         </is>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="13.5">
@@ -523,10 +540,10 @@
         </is>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
@@ -534,10 +551,10 @@
         </is>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="13.5">
@@ -550,10 +567,10 @@
         </is>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
@@ -561,10 +578,10 @@
         </is>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="13.5">
@@ -577,7 +594,7 @@
         </is>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -590,7 +607,7 @@
         </is>
       </c>
       <c r="F14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -608,7 +625,7 @@
         </is>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -621,7 +638,7 @@
         </is>
       </c>
       <c r="F15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -639,20 +656,18 @@
         </is>
       </c>
       <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>BSS123</t>
-        </is>
-      </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
           <t>N-Channel 100V 170mA (Ta) 360mW (Ta) Surface Mount SOT-23-3</t>
         </is>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -685,7 +700,7 @@
         </is>
       </c>
       <c r="F17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -716,7 +731,7 @@
         </is>
       </c>
       <c r="F18" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
@@ -725,64 +740,62 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="13.5">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>R11, R12, R18, R23, R25, R30, R31</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>AC0603FR-071KL</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>1 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
-        </is>
-      </c>
-      <c r="F19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>311-1KLDCT-ND</t>
-        </is>
+      <c r="A19" s="4">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>Q7</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Vishay</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="5" t="inlineStr">
+        <is>
+          <t>P-Channel 60 V 3.2A (Ta) 1.5W (Ta) Surface Mount PowerPAK® SO-8</t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="13.5">
       <c r="A20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>R13</t>
+          <t>R11, R12, R18, R23, R25, R30, R31</t>
         </is>
       </c>
       <c r="C20" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>AC0603FR-071K8L</t>
+          <t>AC0603FR-071KL</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>1.8 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>1 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>311-1.8KLDCT-ND</t>
+          <t>311-1KLDCT-ND</t>
         </is>
       </c>
     </row>
@@ -792,28 +805,28 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R14</t>
+          <t>R13</t>
         </is>
       </c>
       <c r="C21" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>AC0603FR-073K3L</t>
+          <t>AC0603FR-071K8L</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>3.3 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>1.8 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>YAG3605CT-ND</t>
+          <t>311-1.8KLDCT-ND</t>
         </is>
       </c>
     </row>
@@ -823,90 +836,90 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R15</t>
+          <t>R14</t>
         </is>
       </c>
       <c r="C22" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>AC0603FR-0727KL</t>
+          <t>AC0603FR-073K3L</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>27 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>3.3 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>YAG3585CT-ND</t>
+          <t>YAG3605CT-ND</t>
         </is>
       </c>
     </row>
     <row r="23" spans="1:7" ht="13.5">
       <c r="A23">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>R1, R4, R7, R10, R16, R17, R19, R24, R28, R29, R32, R33, R34, R35, R36, R37</t>
+          <t>R15</t>
         </is>
       </c>
       <c r="C23" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>AC0603FR-0710KL</t>
+          <t>AC0603FR-0727KL</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>27 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>311-10KLDCT-ND</t>
+          <t>YAG3585CT-ND</t>
         </is>
       </c>
     </row>
     <row r="24" spans="1:7" ht="13.5">
       <c r="A24">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>R1, R4, R7, R10, R16, R17, R19, R24, R28, R29, R32, R33, R34, R35, R36, R37</t>
         </is>
       </c>
       <c r="C24" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>AC0603FR-07470KL</t>
+          <t>AC0603FR-0710KL</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>470 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>YAG3609CT-ND</t>
+          <t>311-10KLDCT-ND</t>
         </is>
       </c>
     </row>
@@ -916,154 +929,154 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>R2</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>AC0603FR-07470KL</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>470 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+        </is>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>YAG3609CT-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="13.5">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>R20</t>
         </is>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="inlineStr">
+      <c r="C26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="inlineStr">
         <is>
           <t>AC0603FR-072K4L</t>
         </is>
       </c>
-      <c r="E25" s="3" t="inlineStr">
+      <c r="E26" s="3" t="inlineStr">
         <is>
           <t>2.4 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
-      <c r="F25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" t="inlineStr">
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>YAG5724CT-ND</t>
         </is>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13.5">
-      <c r="A26" s="4">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="inlineStr">
+    <row r="27" spans="1:7" ht="13.5">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>R21</t>
         </is>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="4" t="inlineStr">
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="inlineStr">
         <is>
           <t>AC0603FR-07750RL</t>
         </is>
       </c>
-      <c r="E26" s="5" t="inlineStr">
+      <c r="E27" s="5" t="inlineStr">
         <is>
           <t>750 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G26" s="4" t="inlineStr">
+      <c r="F27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4" t="inlineStr">
         <is>
           <t>YAG3628CT-ND</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="13.5">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>R22</t>
-        </is>
-      </c>
-      <c r="C27" s="3" t="inlineStr">
-        <is>
-          <t>StackPole Electronics Inc</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>CSR1206FTR100</t>
-        </is>
-      </c>
-      <c r="E27" s="3" t="inlineStr">
-        <is>
-          <t>100 mOhms ±1% 0.5W, 1/2W Chip Resistor 1206 Current Sense</t>
-        </is>
-      </c>
-      <c r="F27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>CSR1206FTR100CT-ND</t>
         </is>
       </c>
     </row>
     <row r="28" spans="1:7" ht="13.5">
       <c r="A28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>R26, R27</t>
-        </is>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
+          <t>R22</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>StackPole Electronics Inc</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>AC0603FR-0751RL</t>
+          <t>CSR1206FTR100</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>51 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>100 mOhms ±1% 0.5W, 1/2W Chip Resistor 1206 Current Sense</t>
         </is>
       </c>
       <c r="F28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>YAG3617CT-ND</t>
+          <t>CSR1206FTR100CT-ND</t>
         </is>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13.5">
       <c r="A29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R3</t>
+          <t>R26, R27</t>
         </is>
       </c>
       <c r="C29" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>AC0603FR-07150KL</t>
+          <t>AC0603FR-0751RL</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>150 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>51 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>YAG3567CT-ND</t>
+          <t>YAG3617CT-ND</t>
         </is>
       </c>
     </row>
@@ -1073,185 +1086,183 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>R5</t>
+          <t>R3</t>
         </is>
       </c>
       <c r="C30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>AC0603FR-07100KL</t>
+          <t>AC0603FR-07150KL</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+          <t>150 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
       <c r="F30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>311-100KLDCT-ND</t>
+          <t>YAG3567CT-ND</t>
         </is>
       </c>
     </row>
     <row r="31" spans="1:7" ht="13.5">
       <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>R5</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>AC0603FR-07100KL</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>100 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
+        </is>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>311-100KLDCT-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="13.5">
+      <c r="A32">
         <v>2</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>R8, R9</t>
         </is>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="inlineStr">
+      <c r="C32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>AC0603FR-07470RL</t>
         </is>
       </c>
-      <c r="E31" s="3" t="inlineStr">
+      <c r="E32" s="3" t="inlineStr">
         <is>
           <t>470 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric)</t>
         </is>
       </c>
-      <c r="F31" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" t="inlineStr">
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>311-470LDCT-ND</t>
         </is>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.5">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="B32" s="6" t="inlineStr">
+    <row r="33" spans="1:7" ht="13.5">
+      <c r="A33" s="6">
+        <v>1</v>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
         <is>
           <t>U1</t>
         </is>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="6" t="inlineStr">
+      <c r="D33" s="6" t="inlineStr">
         <is>
           <t>STM32F042K6T6</t>
         </is>
       </c>
-      <c r="E32" s="7" t="inlineStr">
+      <c r="E33" s="7" t="inlineStr">
         <is>
           <t>STM32F0 uC IC 32-Bit 48Mhz 32KB (32K x 8) FLASH 32-LQFP (7x7)</t>
         </is>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G32" s="6" t="inlineStr">
+      <c r="F33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6" t="inlineStr">
         <is>
           <t>497-14647-ND</t>
-        </is>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="13.5">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>U2</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>BD62120AEFJ-E2</t>
-        </is>
-      </c>
-      <c r="E33" s="3" t="inlineStr">
-        <is>
-          <t>Motor Driver DMOS On/Off 8-HTSOP-J</t>
-        </is>
-      </c>
-      <c r="F33" t="s">
-        <v>2</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>BD62120AEFJ-E2CT-ND</t>
         </is>
       </c>
     </row>
     <row r="34" spans="1:7" ht="13.5">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>U3, U4</t>
+          <t>U2</t>
         </is>
       </c>
       <c r="C34" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>H11F1SR2M</t>
+          <t>BD62120AEFJ-E2</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>Optoisolator MOSFET Output 7500Vpk 1 Channel 6-SMD</t>
+          <t>Motor Driver DMOS On/Off 8-HTSOP-J</t>
         </is>
       </c>
       <c r="F34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>H11F1SR2MCT-ND</t>
+          <t>BD62120AEFJ-E2CT-ND</t>
         </is>
       </c>
     </row>
     <row r="35" spans="1:7" ht="13.5">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>U5</t>
-        </is>
-      </c>
-      <c r="C35" s="3" t="inlineStr">
-        <is>
-          <t>MPS Inc</t>
-        </is>
+          <t>U3, U4</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>MP26123DR-LF-Z</t>
+          <t>H11F1SR2M</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>Charger IC Lithium-Ion 16-QFN (4x4)</t>
+          <t>Optoisolator MOSFET Output 7500Vpk 1 Channel 6-SMD</t>
         </is>
       </c>
       <c r="F35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1589-1609-1-ND</t>
+          <t>H11F1SR2MCT-ND</t>
         </is>
       </c>
     </row>
@@ -1261,30 +1272,30 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>U6</t>
+          <t>U5</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Amphenol</t>
+          <t>MPS Inc</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>NHQ103B375T10</t>
+          <t>MP26123DR-LF-Z</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>NTC Thermistor 10k 1206 (3216 Metric)</t>
+          <t>Charger IC Lithium-Ion 16-QFN (4x4)</t>
         </is>
       </c>
       <c r="F36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>235-1109-1-ND</t>
+          <t>1589-1609-1-ND</t>
         </is>
       </c>
     </row>
@@ -1294,30 +1305,30 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>U7</t>
+          <t>U6</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>PUI Audio Inc. </t>
+          <t>Amphenol</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>SMT-0440-S-R</t>
+          <t>NHQ103B375T10</t>
         </is>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>Buzzers 3V 90mA 4kHz 70dB @ 3V, 10cm SMD</t>
+          <t>NTC Thermistor 10k 1206 (3216 Metric)</t>
         </is>
       </c>
       <c r="F37" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>668-1488-1-ND</t>
+          <t>235-1109-1-ND</t>
         </is>
       </c>
     </row>
@@ -1327,30 +1338,30 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>U8</t>
+          <t>U7</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Vishay Siliconix</t>
+          <t>PUI Audio Inc. </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>SI7465DP-T1-E3</t>
+          <t>SMT-0440-S-R</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>P-Channel 60V 3.2A (Ta) 1.5W (Ta) Surface Mount PowerPAK® SO-8</t>
+          <t>Buzzers 3V 90mA 4kHz 70dB @ 3V, 10cm SMD</t>
         </is>
       </c>
       <c r="F38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>SI7465DP-T1-E3CT-ND</t>
+          <t>668-1488-1-ND</t>
         </is>
       </c>
     </row>
@@ -1360,31 +1371,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>U10</t>
+          <t>U8</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>Texas Instruments</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>TPS630702RNMT</t>
-        </is>
+          <t>Vishay Siliconix</t>
+        </is>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>Buck-Boost SPS Positive Adjustable 2.5V 2A</t>
+          <t>P-Channel 60V 3.2A (Ta) 1.5W (Ta) Surface Mount PowerPAK® SO-8</t>
         </is>
       </c>
       <c r="F39" t="s">
-        <v>2</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>296-TPS630702RNMTCT-ND</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="13.5">
@@ -1393,28 +1400,61 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>U10</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>Texas Instruments</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>TPS630702RNMT</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>Buck-Boost SPS Positive Adjustable 2.5V 2A</t>
+        </is>
+      </c>
+      <c r="F40" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>296-TPS630702RNMTCT-ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="13.5">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>Y1</t>
         </is>
       </c>
-      <c r="C40" s="3" t="inlineStr">
+      <c r="C41" s="3" t="inlineStr">
         <is>
           <t>ECS Inc.</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>ECS-160-10-36Q-ES-TR</t>
         </is>
       </c>
-      <c r="E40" s="3" t="inlineStr">
+      <c r="E41" s="3" t="inlineStr">
         <is>
           <t>16MHz ±30ppm Crystal 10pF 80 Ohms 4-SMD, No Lead</t>
         </is>
       </c>
-      <c r="F40" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" t="inlineStr">
+      <c r="F41" t="s">
+        <v>1</v>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>XC2181CT-ND</t>
         </is>
@@ -1445,8 +1485,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -1473,8 +1512,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="9.142307692307693"/>
-    <col min="2" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>